<commit_message>
updated graphs, added harem in tools formats
</commit_message>
<xml_diff>
--- a/graphs/f-measure by class/f-measure by entities.xlsx
+++ b/graphs/f-measure by class/f-measure by entities.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\ner-re-pt\graphs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\ner-re-pt\graphs\f-measure by class\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="SIGARRA" sheetId="1" r:id="rId1"/>
@@ -406,48 +406,6 @@
   <dxfs count="29">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -658,13 +616,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -675,6 +626,55 @@
           <color theme="4" tint="0.39997558519241921"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -827,28 +827,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>89.69</c:v>
+                  <c:v>91.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.1</c:v>
+                  <c:v>32.96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.59</c:v>
+                  <c:v>74.87</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.64</c:v>
+                  <c:v>67.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.88</c:v>
+                  <c:v>82.56</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.97</c:v>
+                  <c:v>75.61</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94.79</c:v>
+                  <c:v>94.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.08</c:v>
+                  <c:v>91.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,28 +922,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>96.7</c:v>
+                  <c:v>98.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.42</c:v>
+                  <c:v>35.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.430000000000007</c:v>
+                  <c:v>76.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.989999999999995</c:v>
+                  <c:v>67.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.22</c:v>
+                  <c:v>91.85</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>77.36</c:v>
+                  <c:v>75.47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.48</c:v>
+                  <c:v>96.37</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93.22</c:v>
+                  <c:v>93.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,28 +1017,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>93.49</c:v>
+                  <c:v>94.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.67</c:v>
+                  <c:v>32.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.06</c:v>
+                  <c:v>71.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.73</c:v>
+                  <c:v>63.51</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.3</c:v>
+                  <c:v>78.569999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.16</c:v>
+                  <c:v>70.37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93.37</c:v>
+                  <c:v>93.51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90.75</c:v>
+                  <c:v>91.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,28 +1112,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>90.16</c:v>
+                  <c:v>92.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.29</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.3</c:v>
+                  <c:v>54.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.97</c:v>
+                  <c:v>44.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54.62</c:v>
+                  <c:v>57.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.87</c:v>
+                  <c:v>44.44</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88.24</c:v>
+                  <c:v>89.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77.59</c:v>
+                  <c:v>69.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1207,28 +1207,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>63.4</c:v>
+                  <c:v>40.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.62</c:v>
+                  <c:v>10.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.02</c:v>
+                  <c:v>31.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.3</c:v>
+                  <c:v>26.73</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.82</c:v>
+                  <c:v>32.020000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.95</c:v>
+                  <c:v>32.43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>68.400000000000006</c:v>
+                  <c:v>47.53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>65.8</c:v>
+                  <c:v>50.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1302,28 +1302,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>71.42</c:v>
+                  <c:v>74.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.24</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.07</c:v>
+                  <c:v>47.17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.48</c:v>
+                  <c:v>30.27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.05</c:v>
+                  <c:v>57.55</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.5</c:v>
+                  <c:v>46.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.47</c:v>
+                  <c:v>73.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>91.94</c:v>
+                  <c:v>63.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,7 +1636,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -8489,13 +8489,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
+      <xdr:colOff>98180</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
+      <xdr:colOff>202955</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -8693,19 +8693,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C70:I103" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C70:I103" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="C70:I103"/>
   <sortState ref="C71:I103">
     <sortCondition ref="C70:C103"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Entity class" dataDxfId="8"/>
-    <tableColumn id="2" name="OpenNLP" dataDxfId="7"/>
-    <tableColumn id="3" name="Stanford CoreNLP" dataDxfId="6"/>
-    <tableColumn id="4" name="spaCy" dataDxfId="5"/>
-    <tableColumn id="5" name="NLTK DT" dataDxfId="4"/>
-    <tableColumn id="6" name="NLTK ME" dataDxfId="3"/>
-    <tableColumn id="7" name="NLTK NB" dataDxfId="2"/>
+    <tableColumn id="1" name="Entity class" dataDxfId="6"/>
+    <tableColumn id="2" name="OpenNLP" dataDxfId="5"/>
+    <tableColumn id="3" name="Stanford CoreNLP" dataDxfId="4"/>
+    <tableColumn id="4" name="spaCy" dataDxfId="3"/>
+    <tableColumn id="5" name="NLTK DT" dataDxfId="2"/>
+    <tableColumn id="6" name="NLTK ME" dataDxfId="1"/>
+    <tableColumn id="7" name="NLTK NB" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9010,8 +9010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:I13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9052,22 +9052,22 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>89.69</v>
+        <v>91.64</v>
       </c>
       <c r="E6" s="1">
-        <v>96.7</v>
+        <v>98.02</v>
       </c>
       <c r="F6" s="1">
-        <v>93.49</v>
+        <v>94.62</v>
       </c>
       <c r="G6" s="1">
-        <v>90.16</v>
+        <v>92.85</v>
       </c>
       <c r="H6" s="1">
-        <v>63.4</v>
+        <v>40.03</v>
       </c>
       <c r="I6" s="1">
-        <v>71.42</v>
+        <v>74.849999999999994</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
@@ -9075,22 +9075,22 @@
         <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>37.1</v>
+        <v>32.96</v>
       </c>
       <c r="E7" s="1">
-        <v>33.42</v>
+        <v>35.18</v>
       </c>
       <c r="F7" s="1">
-        <v>32.67</v>
+        <v>32.65</v>
       </c>
       <c r="G7" s="1">
-        <v>11.29</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H7" s="1">
-        <v>14.62</v>
+        <v>10.29</v>
       </c>
       <c r="I7" s="1">
-        <v>3.24</v>
+        <v>6.02</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
@@ -9098,22 +9098,22 @@
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>75.59</v>
+        <v>74.87</v>
       </c>
       <c r="E8" s="1">
-        <v>77.430000000000007</v>
+        <v>76.02</v>
       </c>
       <c r="F8" s="1">
-        <v>72.06</v>
+        <v>71.3</v>
       </c>
       <c r="G8" s="1">
-        <v>53.3</v>
+        <v>54.61</v>
       </c>
       <c r="H8" s="1">
-        <v>51.02</v>
+        <v>31.19</v>
       </c>
       <c r="I8" s="1">
-        <v>44.07</v>
+        <v>47.17</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -9121,22 +9121,22 @@
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>66.64</v>
+        <v>67.44</v>
       </c>
       <c r="E9" s="1">
-        <v>66.989999999999995</v>
+        <v>67.52</v>
       </c>
       <c r="F9" s="1">
-        <v>60.73</v>
+        <v>63.51</v>
       </c>
       <c r="G9" s="1">
-        <v>43.97</v>
+        <v>44.2</v>
       </c>
       <c r="H9" s="1">
-        <v>43.3</v>
+        <v>26.73</v>
       </c>
       <c r="I9" s="1">
-        <v>22.48</v>
+        <v>30.27</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
@@ -9144,22 +9144,22 @@
         <v>4</v>
       </c>
       <c r="D10" s="1">
-        <v>81.88</v>
+        <v>82.56</v>
       </c>
       <c r="E10" s="1">
-        <v>91.22</v>
+        <v>91.85</v>
       </c>
       <c r="F10" s="1">
-        <v>77.3</v>
+        <v>78.569999999999993</v>
       </c>
       <c r="G10" s="1">
-        <v>54.62</v>
+        <v>57.1</v>
       </c>
       <c r="H10" s="1">
-        <v>51.82</v>
+        <v>32.020000000000003</v>
       </c>
       <c r="I10" s="1">
-        <v>58.05</v>
+        <v>57.55</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
@@ -9167,22 +9167,22 @@
         <v>5</v>
       </c>
       <c r="D11" s="1">
-        <v>74.97</v>
+        <v>75.61</v>
       </c>
       <c r="E11" s="1">
-        <v>77.36</v>
+        <v>75.47</v>
       </c>
       <c r="F11" s="1">
-        <v>69.16</v>
+        <v>70.37</v>
       </c>
       <c r="G11" s="1">
-        <v>56.87</v>
+        <v>44.44</v>
       </c>
       <c r="H11" s="1">
-        <v>55.95</v>
+        <v>32.43</v>
       </c>
       <c r="I11" s="1">
-        <v>43.5</v>
+        <v>46.25</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
@@ -9190,22 +9190,22 @@
         <v>6</v>
       </c>
       <c r="D12" s="1">
-        <v>94.79</v>
+        <v>94.59</v>
       </c>
       <c r="E12" s="1">
-        <v>96.48</v>
+        <v>96.37</v>
       </c>
       <c r="F12" s="1">
-        <v>93.37</v>
+        <v>93.51</v>
       </c>
       <c r="G12" s="1">
-        <v>88.24</v>
+        <v>89.3</v>
       </c>
       <c r="H12" s="1">
-        <v>68.400000000000006</v>
+        <v>47.53</v>
       </c>
       <c r="I12" s="1">
-        <v>72.47</v>
+        <v>73.08</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
@@ -9213,27 +9213,27 @@
         <v>7</v>
       </c>
       <c r="D13" s="1">
-        <v>92.08</v>
+        <v>91.76</v>
       </c>
       <c r="E13" s="1">
-        <v>93.22</v>
+        <v>93.81</v>
       </c>
       <c r="F13" s="1">
-        <v>90.75</v>
+        <v>91.52</v>
       </c>
       <c r="G13" s="1">
-        <v>77.59</v>
+        <v>69.14</v>
       </c>
       <c r="H13" s="1">
-        <v>65.8</v>
+        <v>50.78</v>
       </c>
       <c r="I13" s="1">
-        <v>91.94</v>
+        <v>63.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -9245,7 +9245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="F69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>

</xml_diff>